<commit_message>
added millis() to take over if interrupt doesn't work
</commit_message>
<xml_diff>
--- a/LCD mapping.xlsx
+++ b/LCD mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madis\Desktop\NTP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/001aa055a3bf4321/Documents/Arduino/NTP_clock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C5A0E5-3ECC-420E-8B47-1428CADC6A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{83C5A0E5-3ECC-420E-8B47-1428CADC6A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8DF48370-FDDD-4DAA-8960-896D31AD95B6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{E4A7D367-EF4E-4250-8CCB-DE9F4621B5AF}"/>
+    <workbookView minimized="1" xWindow="3600" yWindow="1215" windowWidth="6960" windowHeight="10425" xr2:uid="{E4A7D367-EF4E-4250-8CCB-DE9F4621B5AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
   <si>
     <t>D0</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>LCD PIN</t>
+  </si>
+  <si>
+    <t>HEARTB</t>
   </si>
 </sst>
 </file>
@@ -935,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB2D8A7-78A0-419A-819C-6D24D3E2DD68}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,6 +966,9 @@
       <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="J1">
+        <v>14</v>
+      </c>
       <c r="K1" s="5">
         <v>6</v>
       </c>
@@ -974,6 +980,9 @@
       </c>
       <c r="N1" s="5">
         <v>5</v>
+      </c>
+      <c r="O1">
+        <v>1</v>
       </c>
       <c r="Q1" s="47"/>
       <c r="R1" s="47"/>
@@ -993,6 +1002,9 @@
       <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
       <c r="K2" s="23">
         <v>7</v>
       </c>
@@ -1004,6 +1016,9 @@
       </c>
       <c r="N2" s="29">
         <v>4</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
       </c>
       <c r="Q2" s="47"/>
       <c r="R2" s="47"/>
@@ -1023,6 +1038,9 @@
       <c r="F3" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
       <c r="K3" s="7">
         <v>8</v>
       </c>
@@ -1033,6 +1051,9 @@
         <v>16</v>
       </c>
       <c r="N3" s="25">
+        <v>3</v>
+      </c>
+      <c r="O3">
         <v>3</v>
       </c>
       <c r="Q3" s="47"/>
@@ -1053,6 +1074,9 @@
       <c r="F4" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
       <c r="K4" s="7">
         <v>9</v>
       </c>
@@ -1064,6 +1088,9 @@
       </c>
       <c r="N4" s="32">
         <v>2</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
       </c>
       <c r="Q4" s="47"/>
       <c r="R4" s="47"/>
@@ -1086,6 +1113,9 @@
       <c r="G5" t="s">
         <v>66</v>
       </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
       <c r="K5" s="7">
         <v>10</v>
       </c>
@@ -1097,6 +1127,9 @@
       </c>
       <c r="N5" s="34">
         <v>1</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
       </c>
       <c r="Q5" s="47"/>
       <c r="R5" s="47"/>
@@ -1118,6 +1151,9 @@
       <c r="F6" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
       <c r="K6" s="21">
         <v>11</v>
       </c>
@@ -1129,6 +1165,9 @@
       </c>
       <c r="N6" s="36">
         <v>0</v>
+      </c>
+      <c r="O6">
+        <v>6</v>
       </c>
       <c r="Q6" s="47"/>
       <c r="R6" s="49"/>
@@ -1150,6 +1189,9 @@
       <c r="F7" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
       <c r="K7" s="19">
         <v>12</v>
       </c>
@@ -1161,6 +1203,9 @@
       </c>
       <c r="N7" s="38" t="s">
         <v>28</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
       </c>
       <c r="Q7" s="47"/>
       <c r="R7" s="47"/>
@@ -1180,6 +1225,9 @@
       <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
       <c r="K8" s="30">
         <v>13</v>
       </c>
@@ -1191,6 +1239,9 @@
       </c>
       <c r="N8" s="40" t="s">
         <v>27</v>
+      </c>
+      <c r="O8">
+        <v>8</v>
       </c>
       <c r="Q8" s="47"/>
       <c r="R8" s="47"/>
@@ -1212,6 +1263,9 @@
       <c r="F9" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
       <c r="K9" s="30">
         <v>14</v>
       </c>
@@ -1223,6 +1277,9 @@
       </c>
       <c r="N9" s="27" t="s">
         <v>26</v>
+      </c>
+      <c r="O9">
+        <v>9</v>
       </c>
       <c r="Q9" s="47"/>
       <c r="R9" s="47"/>
@@ -1244,6 +1301,9 @@
       <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
       <c r="K10" s="6" t="s">
         <v>63</v>
       </c>
@@ -1255,6 +1315,9 @@
       </c>
       <c r="N10" s="16" t="s">
         <v>25</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
       </c>
       <c r="Q10" s="47"/>
       <c r="R10" s="47"/>
@@ -1275,6 +1338,9 @@
       </c>
       <c r="F11" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>47</v>
@@ -1284,6 +1350,9 @@
       <c r="N11" s="14" t="s">
         <v>24</v>
       </c>
+      <c r="O11">
+        <v>11</v>
+      </c>
       <c r="Q11" s="47"/>
       <c r="R11" s="47"/>
     </row>
@@ -1302,13 +1371,21 @@
       <c r="F12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
       <c r="K12" s="30" t="s">
         <v>53</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="10"/>
+      <c r="M12" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="N12" s="30" t="s">
         <v>23</v>
+      </c>
+      <c r="O12">
+        <v>12</v>
       </c>
       <c r="Q12" s="47"/>
       <c r="R12" s="47"/>
@@ -1328,13 +1405,18 @@
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
       <c r="K13" s="6" t="s">
         <v>64</v>
       </c>
       <c r="L13" s="3"/>
-      <c r="M13" s="10"/>
       <c r="N13" s="30" t="s">
         <v>22</v>
+      </c>
+      <c r="O13">
+        <v>13</v>
       </c>
       <c r="Q13" s="47"/>
       <c r="R13" s="47"/>
@@ -1355,6 +1437,9 @@
       </c>
       <c r="F14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
       </c>
       <c r="K14" s="41" t="s">
         <v>48</v>
@@ -1363,6 +1448,9 @@
       <c r="M14" s="10"/>
       <c r="N14" s="9" t="s">
         <v>65</v>
+      </c>
+      <c r="O14">
+        <v>14</v>
       </c>
       <c r="Q14" s="47"/>
       <c r="R14" s="47"/>

</xml_diff>